<commit_message>
update config and categroy data file
</commit_message>
<xml_diff>
--- a/data/news_category_eng.xlsx
+++ b/data/news_category_eng.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaeb/news/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5D9722-C151-F84B-A9FE-C4D8CB1E4D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4141210-4635-3942-B5C9-6A1E32AE7A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="500" windowWidth="18840" windowHeight="20500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="500" windowWidth="18840" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="policy" sheetId="8" r:id="rId1"/>
+    <sheet name="politics" sheetId="8" r:id="rId1"/>
     <sheet name="economy" sheetId="9" r:id="rId2"/>
     <sheet name="international" sheetId="10" r:id="rId3"/>
     <sheet name="society" sheetId="11" r:id="rId4"/>
@@ -1396,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1412,9 +1412,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1719,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2392EDE6-39C3-0C40-88D1-A51087810B7F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1834,7 +1831,7 @@
       <c r="H4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>283</v>
       </c>
     </row>
@@ -1863,7 +1860,7 @@
       <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>284</v>
       </c>
     </row>
@@ -1892,7 +1889,7 @@
       <c r="H6" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="2" t="s">
         <v>285</v>
       </c>
     </row>
@@ -1921,7 +1918,7 @@
       <c r="H7" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="2" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2052,7 +2049,7 @@
       <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2081,7 +2078,7 @@
       <c r="H4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>288</v>
       </c>
     </row>
@@ -2110,7 +2107,7 @@
       <c r="H5" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2139,7 +2136,7 @@
       <c r="H6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="2" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2168,7 +2165,7 @@
       <c r="H7" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="2" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2197,7 +2194,7 @@
       <c r="H8" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="2" t="s">
         <v>292</v>
       </c>
     </row>
@@ -2392,7 +2389,7 @@
       <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2421,7 +2418,7 @@
       <c r="H4" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2450,7 +2447,7 @@
       <c r="H5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2476,7 +2473,7 @@
       <c r="H6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="2" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2502,7 +2499,7 @@
       <c r="H7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2528,7 +2525,7 @@
       <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="2" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2684,7 +2681,7 @@
       <c r="H3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2713,7 +2710,7 @@
       <c r="H4" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2742,7 +2739,7 @@
       <c r="H5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2771,7 +2768,7 @@
       <c r="H6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="2" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2800,7 +2797,7 @@
       <c r="H7" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="2" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2829,7 +2826,7 @@
       <c r="H8" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="2" t="s">
         <v>305</v>
       </c>
     </row>
@@ -2855,7 +2852,7 @@
       <c r="H9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="2" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3052,7 +3049,7 @@
       <c r="H3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3081,7 +3078,7 @@
       <c r="H4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3110,7 +3107,7 @@
       <c r="H5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3469,7 +3466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A241BA-95DA-A947-B24A-65948961B871}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -3558,7 +3555,7 @@
       <c r="H3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="2" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3587,7 +3584,7 @@
       <c r="H4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="2" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3616,7 +3613,7 @@
       <c r="H5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="2" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3645,7 +3642,7 @@
       <c r="H6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="2" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3674,7 +3671,7 @@
       <c r="H7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="2" t="s">
         <v>321</v>
       </c>
     </row>
@@ -3698,7 +3695,7 @@
       <c r="H8" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="2" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3715,7 +3712,7 @@
       <c r="H9" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="2" t="s">
         <v>323</v>
       </c>
     </row>

</xml_diff>